<commit_message>
Tabla clientes (cond + prop) carga (tomar ex. doble dni) - inicio con controller + html inspecciones
</commit_message>
<xml_diff>
--- a/_extras/VTV_DB-MySQL.xlsx
+++ b/_extras/VTV_DB-MySQL.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="59">
   <si>
     <t>personas</t>
   </si>
@@ -223,6 +223,25 @@
   </si>
   <si>
     <t>inspecciones</t>
+  </si>
+  <si>
+    <t>cliente</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">def. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alta</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -485,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -541,12 +560,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -572,6 +585,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -877,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,28 +927,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="H3" s="22"/>
+      <c r="K3" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="24"/>
+      <c r="L3" s="22"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -952,7 +974,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="20" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -975,7 +997,7 @@
       <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1010,7 +1032,7 @@
       <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="20" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1019,11 +1041,11 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
       <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="K9" s="8" t="s">
@@ -1034,17 +1056,17 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="28"/>
+      <c r="H10" s="26"/>
       <c r="K10" s="5"/>
       <c r="L10" s="3" t="s">
         <v>48</v>
@@ -1094,20 +1116,20 @@
       <c r="S13" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U13" s="19" t="s">
+      <c r="U13" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="V13" s="20"/>
+      <c r="V13" s="30"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="G14" s="26" t="s">
+      <c r="C14" s="27"/>
+      <c r="G14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="26"/>
       <c r="O14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1200,23 +1222,23 @@
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="25" t="s">
+      <c r="S18" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="G19" s="26" t="s">
+      <c r="C19" s="26"/>
+      <c r="G19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="S19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1228,7 +1250,7 @@
       <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S20" s="25"/>
+      <c r="S20" s="23"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
@@ -1239,7 +1261,7 @@
       <c r="H21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S21" s="25"/>
+      <c r="S21" s="23"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
@@ -1254,10 +1276,11 @@
       <c r="H22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S22" s="25"/>
+      <c r="S22" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="U13:V13"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="S18:S22"/>
     <mergeCell ref="B9:D9"/>
@@ -1279,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U13" sqref="U13:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,28 +1330,28 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="24"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="G3" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="24"/>
-      <c r="K3" s="24" t="s">
+      <c r="H3" s="22"/>
+      <c r="K3" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="24"/>
+      <c r="L3" s="22"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1354,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="20" t="s">
         <v>30</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1377,7 +1400,7 @@
       <c r="H6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="19" t="s">
         <v>30</v>
       </c>
       <c r="L6" s="3" t="s">
@@ -1412,7 +1435,7 @@
       <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="20" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1421,11 +1444,11 @@
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
       <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="K9" s="8" t="s">
@@ -1436,7 +1459,7 @@
       </c>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1445,10 +1468,10 @@
       <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H10" s="28"/>
+      <c r="H10" s="26"/>
       <c r="K10" s="5"/>
       <c r="L10" s="3" t="s">
         <v>48</v>
@@ -1491,20 +1514,20 @@
       <c r="S13" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="U13" s="19" t="s">
+      <c r="U13" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="V13" s="20"/>
+      <c r="V13" s="30"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="G14" s="26" t="s">
+      <c r="C14" s="27"/>
+      <c r="G14" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="26"/>
       <c r="O14" s="13" t="s">
         <v>35</v>
       </c>
@@ -1594,23 +1617,23 @@
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="25" t="s">
+      <c r="S18" s="23" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="G19" s="26" t="s">
+      <c r="C19" s="26"/>
+      <c r="G19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="28"/>
-      <c r="S19" s="25"/>
+      <c r="H19" s="26"/>
+      <c r="S19" s="23"/>
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="20" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1625,7 +1648,7 @@
       <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="S20" s="25"/>
+      <c r="S20" s="23"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
@@ -1636,7 +1659,7 @@
       <c r="H21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S21" s="25"/>
+      <c r="S21" s="23"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G22" s="11" t="s">
@@ -1645,21 +1668,22 @@
       <c r="H22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="S22" s="25"/>
+      <c r="S22" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="S18:S22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="S18:S22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1668,12 +1692,423 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G2" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="22"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="G3" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="22"/>
+      <c r="K3" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="22"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="G4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="G5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="G6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="G8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="26"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="26"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="R13" s="15"/>
+      <c r="S13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="U13" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="V13" s="30"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="G14" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="26"/>
+      <c r="O14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="V15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S18" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G19" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="H19" s="26"/>
+      <c r="S19" s="23"/>
+    </row>
+    <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="S20" s="23"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S21" s="23"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S22" s="23"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="S18:S22"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G10:H10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Carga auto (valida dominio OK, falta vincular marcas-modelos) - carga inspección (inspector de lista activos) - Empleado puestos desde Enum
</commit_message>
<xml_diff>
--- a/_extras/VTV_DB-MySQL.xlsx
+++ b/_extras/VTV_DB-MySQL.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="57">
   <si>
     <t>personas</t>
   </si>
@@ -72,9 +72,6 @@
     <t>modelo</t>
   </si>
   <si>
-    <t>motor</t>
-  </si>
-  <si>
     <t>marcas</t>
   </si>
   <si>
@@ -88,15 +85,6 @@
   </si>
   <si>
     <t>idModelo</t>
-  </si>
-  <si>
-    <t>motorizacion</t>
-  </si>
-  <si>
-    <t>idMotor</t>
-  </si>
-  <si>
-    <t>inspeciones</t>
   </si>
   <si>
     <t>idInspeccion</t>
@@ -242,6 +230,12 @@
       </rPr>
       <t>Alta</t>
     </r>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>idVersion</t>
   </si>
 </sst>
 </file>
@@ -569,6 +563,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,15 +588,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -899,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13:V13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,25 +921,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="G3" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="22"/>
-      <c r="K3" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L3" s="22"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="K3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
@@ -965,7 +959,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
@@ -975,14 +969,14 @@
       </c>
       <c r="D5" s="3"/>
       <c r="G5" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
@@ -992,33 +986,33 @@
       </c>
       <c r="D6" s="3"/>
       <c r="G6" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="G7" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N7" s="14"/>
     </row>
@@ -1027,29 +1021,29 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="G8" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="K9" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>15</v>
@@ -1063,13 +1057,15 @@
         <v>5</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="K10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1078,22 +1074,24 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>1</v>
@@ -1103,44 +1101,58 @@
       <c r="H12" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="K12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="5"/>
+      <c r="L13" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="O13" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="U13" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="V13" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" s="24"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="G14" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="26"/>
+      <c r="C14" s="30"/>
+      <c r="G14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O14" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U14" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="V14" s="13">
         <v>1</v>
@@ -1157,19 +1169,19 @@
         <v>4</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="V15" s="3">
         <v>2</v>
@@ -1185,16 +1197,16 @@
         <v>17</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="V16" s="3">
         <v>3</v>
@@ -1202,40 +1214,40 @@
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="23" t="s">
-        <v>53</v>
+      <c r="S18" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="G19" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="S19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="G19" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="S19" s="26"/>
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
@@ -1248,35 +1260,35 @@
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S20" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="S20" s="26"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S21" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="S21" s="26"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" s="23"/>
+        <v>22</v>
+      </c>
+      <c r="S22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1303,7 +1315,7 @@
   <dimension ref="B2:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U13" sqref="U13:V13"/>
+      <selection activeCell="K3" sqref="K3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,25 +1342,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="G3" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="22"/>
-      <c r="K3" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="22"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="K3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
@@ -1368,7 +1380,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
@@ -1378,14 +1390,14 @@
       </c>
       <c r="D5" s="3"/>
       <c r="G5" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
@@ -1395,33 +1407,33 @@
       </c>
       <c r="D6" s="3"/>
       <c r="G6" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="G7" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N7" s="14"/>
     </row>
@@ -1430,29 +1442,29 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="G8" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="K9" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>15</v>
@@ -1466,15 +1478,17 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="K10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1483,17 +1497,19 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1501,44 +1517,58 @@
       <c r="H12" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="K12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="5"/>
+      <c r="L13" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="O13" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="U13" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="V13" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" s="24"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="G14" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="26"/>
+      <c r="C14" s="30"/>
+      <c r="G14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O14" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U14" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="V14" s="13">
         <v>1</v>
@@ -1552,25 +1582,25 @@
         <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="V15" s="3">
         <v>2</v>
@@ -1586,16 +1616,16 @@
         <v>17</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="V16" s="3">
         <v>3</v>
@@ -1603,34 +1633,34 @@
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G17" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="23" t="s">
-        <v>53</v>
+      <c r="S18" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="G19" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="S19" s="23"/>
+      <c r="C19" s="29"/>
+      <c r="G19" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="S19" s="26"/>
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="20" t="s">
@@ -1640,35 +1670,35 @@
         <v>1</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S20" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="S20" s="26"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S21" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="S21" s="26"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G22" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" s="23"/>
+        <v>22</v>
+      </c>
+      <c r="S22" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1694,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,25 +1752,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="G3" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="22"/>
-      <c r="K3" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="22"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="K3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="25"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4" s="21" t="s">
@@ -1760,7 +1790,7 @@
         <v>4</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.25">
@@ -1770,14 +1800,14 @@
       </c>
       <c r="D5" s="3"/>
       <c r="G5" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
@@ -1787,33 +1817,33 @@
       </c>
       <c r="D6" s="3"/>
       <c r="G6" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="G7" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="N7" s="14"/>
     </row>
@@ -1822,29 +1852,29 @@
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
       <c r="G8" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="N8" s="14"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
       <c r="G9" s="7"/>
       <c r="H9" s="2"/>
       <c r="K9" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>15</v>
@@ -1858,15 +1888,17 @@
         <v>1</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="K10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="H10" s="26"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,70 +1907,86 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G11" s="10" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="3"/>
+        <v>19</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="K12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K13" s="5"/>
+      <c r="L13" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="O13" s="16" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P13" s="15"/>
       <c r="Q13" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="R13" s="15"/>
       <c r="S13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="U13" s="29" t="s">
-        <v>49</v>
-      </c>
-      <c r="V13" s="30"/>
+        <v>40</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" s="24"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="G14" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="26"/>
+      <c r="B14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="G14" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="29"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="O14" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="Q14" s="13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="U14" s="13" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="V14" s="13">
         <v>1</v>
@@ -1952,25 +2000,25 @@
         <v>1</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="S15" s="18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="V15" s="3">
         <v>2</v>
@@ -1979,7 +2027,7 @@
     <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="3"/>
       <c r="G16" s="3"/>
@@ -1987,16 +2035,16 @@
         <v>17</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="V16" s="3">
         <v>3</v>
@@ -2004,59 +2052,59 @@
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G17" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="S18" s="23" t="s">
-        <v>53</v>
+      <c r="S18" s="26" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G19" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="H19" s="26"/>
-      <c r="S19" s="23"/>
+      <c r="G19" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="S19" s="26"/>
     </row>
     <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G20" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="S20" s="23"/>
+        <v>56</v>
+      </c>
+      <c r="S20" s="26"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="S21" s="23"/>
+        <v>55</v>
+      </c>
+      <c r="S21" s="26"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G22" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="S22" s="23"/>
+        <v>22</v>
+      </c>
+      <c r="S22" s="26"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.25">
@@ -2080,8 +2128,8 @@
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
       <c r="D28" s="7"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.25">
@@ -2101,12 +2149,12 @@
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="S18:S22"/>
     <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Selección de marca-modelo-versión filtrados por Id correspondiente
</commit_message>
<xml_diff>
--- a/_extras/VTV_DB-MySQL.xlsx
+++ b/_extras/VTV_DB-MySQL.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="4" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="5" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="58">
   <si>
     <t>personas</t>
   </si>
@@ -236,6 +237,9 @@
   </si>
   <si>
     <t>idVersion</t>
+  </si>
+  <si>
+    <t>Cliente</t>
   </si>
 </sst>
 </file>
@@ -498,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -588,6 +592,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1702,18 +1709,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B9:D9"/>
     <mergeCell ref="U13:V13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="S18:S22"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="B9:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1724,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,17 +2151,441 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="U13:V13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="S18:S22"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="B9:D9"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="S18:S22"/>
+    <mergeCell ref="G19:H19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:V29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" style="1" customWidth="1"/>
+    <col min="9" max="10" width="2.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" customWidth="1"/>
+    <col min="13" max="14" width="2.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2.7109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="2.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="2.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G2" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="G3" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="K3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" s="25"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="G4" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="G5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="G6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="G7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N7" s="14"/>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="G8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" s="14"/>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="2"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B10" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="31"/>
+      <c r="L11" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" s="15"/>
+      <c r="S13" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" s="24"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="O14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="S14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U14" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="V14" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="29"/>
+      <c r="O15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="V15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="G16" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V16" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S18" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="S19" s="26"/>
+    </row>
+    <row r="20" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="29"/>
+      <c r="S20" s="26"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="S21" s="26"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S22" s="26"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="S18:S22"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G10:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>